<commit_message>
Backlog del Sprint terminado
</commit_message>
<xml_diff>
--- a/02. PLANIFICACION/Backlog Detallado del Producto.xlsx
+++ b/02. PLANIFICACION/Backlog Detallado del Producto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10530" windowHeight="7320" tabRatio="522"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10530" windowHeight="7320" tabRatio="522" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog del Producto" sheetId="8" r:id="rId1"/>
@@ -736,6 +736,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -765,9 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1348,8 +1348,8 @@
   </sheetPr>
   <dimension ref="B1:Q80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1384,14 +1384,14 @@
       </c>
     </row>
     <row r="2" spans="2:17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="40"/>
       <c r="G2" s="40"/>
       <c r="H2" s="35"/>
@@ -1408,14 +1408,14 @@
       </c>
     </row>
     <row r="3" spans="2:17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
       <c r="H3" s="35"/>
@@ -1452,25 +1452,25 @@
       </c>
     </row>
     <row r="5" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="54" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="49" t="s">
+      <c r="G5" s="56"/>
+      <c r="H5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
     </row>
     <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
@@ -1541,7 +1541,7 @@
       <c r="J7" s="8">
         <v>30</v>
       </c>
-      <c r="K7" s="56" t="s">
+      <c r="K7" s="46" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="8">
@@ -1580,7 +1580,7 @@
       <c r="J8" s="8">
         <v>40</v>
       </c>
-      <c r="K8" s="56" t="s">
+      <c r="K8" s="46" t="s">
         <v>33</v>
       </c>
       <c r="L8" s="8">
@@ -1619,7 +1619,7 @@
       <c r="J9" s="8">
         <v>25</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="46" t="s">
         <v>34</v>
       </c>
       <c r="L9" s="8">
@@ -1658,7 +1658,7 @@
       <c r="J10" s="8">
         <v>40</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="46" t="s">
         <v>35</v>
       </c>
       <c r="L10" s="8">
@@ -1697,7 +1697,7 @@
       <c r="J11" s="8">
         <v>40</v>
       </c>
-      <c r="K11" s="56" t="s">
+      <c r="K11" s="46" t="s">
         <v>36</v>
       </c>
       <c r="L11" s="8">
@@ -1736,7 +1736,7 @@
       <c r="J12" s="8">
         <v>40</v>
       </c>
-      <c r="K12" s="56" t="s">
+      <c r="K12" s="46" t="s">
         <v>37</v>
       </c>
       <c r="L12" s="8">
@@ -1775,7 +1775,7 @@
       <c r="J13" s="8">
         <v>10</v>
       </c>
-      <c r="K13" s="56" t="s">
+      <c r="K13" s="46" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="8">
@@ -1814,7 +1814,7 @@
       <c r="J14" s="8">
         <v>10</v>
       </c>
-      <c r="K14" s="56" t="s">
+      <c r="K14" s="46" t="s">
         <v>39</v>
       </c>
       <c r="L14" s="8">
@@ -1853,7 +1853,7 @@
       <c r="J15" s="8">
         <v>10</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="46" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="8">
@@ -2522,7 +2522,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -2997,6 +2997,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ECBD21C84E4C4B48B27A6166FAC051E5" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bb6739421a50b20a8dee76844e41c5f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="100486ed-dfc5-4b43-a390-ed80e6fa3473" xmlns:ns3="3245187f-2b70-4b96-af74-b65b25777eca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="093860096c687094a446cbcfc6e32844" ns2:_="" ns3:_="">
     <xsd:import namespace="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
@@ -3173,31 +3197,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959CDC92-A2D2-49A2-AF46-B019E8B2B1B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3214,37 +3247,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>